<commit_message>
NitrogenProduction now reacts to action events to mirror SedimentProduction2.
</commit_message>
<xml_diff>
--- a/cmd/cremexplorer/testdata/testInputExcelDataSet.xlsx
+++ b/cmd/cremexplorer/testdata/testInputExcelDataSet.xlsx
@@ -4,11 +4,12 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9303"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12375"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12375" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="PlanningUnits" sheetId="1" r:id="rId1"/>
     <sheet name="Gullies" sheetId="2" r:id="rId2"/>
+    <sheet name="ParentSoils" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="145621"/>
   <extLst>
@@ -22,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="26">
   <si>
     <t>Identifier</t>
   </si>
@@ -76,6 +77,30 @@
   </si>
   <si>
     <t>HillslopeDistance</t>
+  </si>
+  <si>
+    <t>PlanningUnit</t>
+  </si>
+  <si>
+    <t>SoilSource</t>
+  </si>
+  <si>
+    <t>TotalNitrogen</t>
+  </si>
+  <si>
+    <t>TotalCarbon</t>
+  </si>
+  <si>
+    <t>DeltaCarbon</t>
+  </si>
+  <si>
+    <t>Gully</t>
+  </si>
+  <si>
+    <t>Hillslope</t>
+  </si>
+  <si>
+    <t>Riparian</t>
   </si>
 </sst>
 </file>
@@ -910,7 +935,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -920,8 +945,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M13" sqref="M13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I31" sqref="I31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1384,4 +1409,323 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E17"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G4" sqref="G4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="12" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>17</v>
+      </c>
+      <c r="B2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2">
+        <v>7.7499999999999999E-2</v>
+      </c>
+      <c r="D2">
+        <v>2.5024999999999999</v>
+      </c>
+      <c r="E2">
+        <f>D2*0.6</f>
+        <v>1.5014999999999998</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>17</v>
+      </c>
+      <c r="B3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C3">
+        <v>0.13</v>
+      </c>
+      <c r="D3">
+        <v>1.846666667</v>
+      </c>
+      <c r="E3">
+        <v>0.44323716600000002</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>17</v>
+      </c>
+      <c r="B4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C4">
+        <v>8.3992857000000004E-2</v>
+      </c>
+      <c r="D4">
+        <v>0.98380449000000003</v>
+      </c>
+      <c r="E4">
+        <f>D4*0.6</f>
+        <v>0.590282694</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>18</v>
+      </c>
+      <c r="B5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C5">
+        <v>0.104</v>
+      </c>
+      <c r="D5">
+        <v>1.2593333330000001</v>
+      </c>
+      <c r="E5">
+        <f>D5*0.6</f>
+        <v>0.75559999980000003</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>18</v>
+      </c>
+      <c r="B6" t="s">
+        <v>24</v>
+      </c>
+      <c r="C6">
+        <v>0.140555556</v>
+      </c>
+      <c r="D6">
+        <v>1.795212732</v>
+      </c>
+      <c r="E6">
+        <v>0.41816441999999998</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>18</v>
+      </c>
+      <c r="B7" t="s">
+        <v>25</v>
+      </c>
+      <c r="C7">
+        <v>8.4071434E-2</v>
+      </c>
+      <c r="D7">
+        <v>0.98553754800000004</v>
+      </c>
+      <c r="E7">
+        <f>D7*0.6</f>
+        <v>0.59132252880000002</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>19</v>
+      </c>
+      <c r="B8" t="s">
+        <v>24</v>
+      </c>
+      <c r="C8">
+        <v>0.154</v>
+      </c>
+      <c r="D8">
+        <v>2.04</v>
+      </c>
+      <c r="E8">
+        <v>0.38100310199999998</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>19</v>
+      </c>
+      <c r="B9" t="s">
+        <v>25</v>
+      </c>
+      <c r="C9">
+        <v>9.0518973000000003E-2</v>
+      </c>
+      <c r="D9">
+        <v>1.2294546129999999</v>
+      </c>
+      <c r="E9">
+        <f>D9*0.6</f>
+        <v>0.73767276779999991</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>20</v>
+      </c>
+      <c r="B10" t="s">
+        <v>24</v>
+      </c>
+      <c r="C10">
+        <v>0.12842857099999999</v>
+      </c>
+      <c r="D10">
+        <v>1.929857143</v>
+      </c>
+      <c r="E10">
+        <v>0.44999999999999996</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>20</v>
+      </c>
+      <c r="B11" t="s">
+        <v>25</v>
+      </c>
+      <c r="C11">
+        <v>0.104666667</v>
+      </c>
+      <c r="D11">
+        <v>1.2633333330000001</v>
+      </c>
+      <c r="E11">
+        <f>D11*0.6</f>
+        <v>0.75799999979999999</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>21</v>
+      </c>
+      <c r="B12" t="s">
+        <v>24</v>
+      </c>
+      <c r="C12">
+        <v>0.14676470599999999</v>
+      </c>
+      <c r="D12">
+        <v>1.9875084030000001</v>
+      </c>
+      <c r="E12">
+        <v>0.44999999999999996</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>21</v>
+      </c>
+      <c r="B13" t="s">
+        <v>25</v>
+      </c>
+      <c r="C13">
+        <v>0.100666667</v>
+      </c>
+      <c r="D13">
+        <v>1.2224888890000001</v>
+      </c>
+      <c r="E13">
+        <f>D13*0.6</f>
+        <v>0.7334933334</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>22</v>
+      </c>
+      <c r="B14" t="s">
+        <v>24</v>
+      </c>
+      <c r="C14">
+        <v>0.13919797</v>
+      </c>
+      <c r="D14">
+        <v>1.802498731</v>
+      </c>
+      <c r="E14">
+        <v>0.44999999999999996</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>22</v>
+      </c>
+      <c r="B15" t="s">
+        <v>25</v>
+      </c>
+      <c r="C15">
+        <v>0.115166667</v>
+      </c>
+      <c r="D15">
+        <v>1.3866666670000001</v>
+      </c>
+      <c r="E15">
+        <f>D15*0.6</f>
+        <v>0.83200000019999998</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>23</v>
+      </c>
+      <c r="B16" t="s">
+        <v>24</v>
+      </c>
+      <c r="C16">
+        <v>0.09</v>
+      </c>
+      <c r="D16">
+        <v>1.5</v>
+      </c>
+      <c r="E16">
+        <v>0.444230772</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>23</v>
+      </c>
+      <c r="B17" t="s">
+        <v>25</v>
+      </c>
+      <c r="C17">
+        <v>9.6666666999999998E-2</v>
+      </c>
+      <c r="D17">
+        <v>1.1777777780000001</v>
+      </c>
+      <c r="E17">
+        <f>D17*0.6</f>
+        <v>0.70666666680000001</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Further fixes to NitrogenProduction variable value calculation.
</commit_message>
<xml_diff>
--- a/cmd/cremexplorer/testdata/testInputExcelDataSet.xlsx
+++ b/cmd/cremexplorer/testdata/testInputExcelDataSet.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9303"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12375" activeTab="2"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="PlanningUnits" sheetId="1" r:id="rId1"/>
@@ -16,6 +16,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -94,20 +95,20 @@
     <t>DeltaCarbon</t>
   </si>
   <si>
+    <t>Hillslope</t>
+  </si>
+  <si>
+    <t>Riparian</t>
+  </si>
+  <si>
     <t>Gully</t>
-  </si>
-  <si>
-    <t>Hillslope</t>
-  </si>
-  <si>
-    <t>Riparian</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -238,6 +239,13 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -540,7 +548,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="42">
+  <cellStyleXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
@@ -583,13 +591,15 @@
     <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="42"/>
   </cellXfs>
-  <cellStyles count="42">
+  <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
     <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
     <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
@@ -627,6 +637,7 @@
     <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
     <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="42"/>
     <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
     <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
     <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
@@ -946,7 +957,7 @@
   <dimension ref="A1:O8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I31" sqref="I31"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -967,7 +978,7 @@
     <col min="15" max="15" width="16.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1014,7 +1025,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>17</v>
       </c>
@@ -1048,20 +1059,20 @@
       <c r="K2">
         <v>151005</v>
       </c>
-      <c r="L2">
-        <v>596613</v>
+      <c r="L2" s="2">
+        <v>730809.75</v>
       </c>
       <c r="M2">
-        <v>8.897474000000001E-2</v>
+        <v>1.1271389999999999E-2</v>
       </c>
       <c r="N2">
-        <v>25583039.881979998</v>
+        <v>236740.80685200001</v>
       </c>
       <c r="O2">
-        <v>50817.812252999996</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+        <v>20820.920407000001</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>18</v>
       </c>
@@ -1095,20 +1106,20 @@
       <c r="K3">
         <v>178202</v>
       </c>
-      <c r="L3">
-        <v>4943321</v>
+      <c r="L3" s="2">
+        <v>3539855</v>
       </c>
       <c r="M3">
-        <v>7.2086440000000002E-2</v>
+        <v>5.3059300000000004E-2</v>
       </c>
       <c r="N3">
-        <v>544975934.25622094</v>
+        <v>13487645.42692</v>
       </c>
       <c r="O3">
-        <v>101256.110996</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+        <v>101270.24266600001</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>19</v>
       </c>
@@ -1142,20 +1153,20 @@
       <c r="K4">
         <v>69012.7</v>
       </c>
-      <c r="L4">
-        <v>2534543</v>
+      <c r="L4" s="2">
+        <v>868235.5</v>
       </c>
       <c r="M4">
-        <v>0.27841275999999998</v>
+        <v>0.11499482999999999</v>
       </c>
       <c r="N4">
-        <v>130351037.04685701</v>
+        <v>491633.18317400001</v>
       </c>
       <c r="O4">
-        <v>67849.539772999997</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+        <v>18010.090768999999</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>20</v>
       </c>
@@ -1189,20 +1200,20 @@
       <c r="K5">
         <v>70059.899999999994</v>
       </c>
-      <c r="L5">
-        <v>84206</v>
+      <c r="L5" s="2">
+        <v>0</v>
       </c>
       <c r="M5">
-        <v>1.9587599999999999E-3</v>
+        <v>0</v>
       </c>
       <c r="N5">
-        <v>1388742.8668480001</v>
+        <v>0</v>
       </c>
       <c r="O5">
-        <v>31142.216537</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>21</v>
       </c>
@@ -1236,20 +1247,20 @@
       <c r="K6">
         <v>96535.1</v>
       </c>
-      <c r="L6">
-        <v>449509</v>
+      <c r="L6" s="2">
+        <v>0</v>
       </c>
       <c r="M6">
-        <v>0.10921844</v>
+        <v>0</v>
       </c>
       <c r="N6">
-        <v>10451836.278557001</v>
+        <v>0</v>
       </c>
       <c r="O6">
-        <v>63657.885459999998</v>
-      </c>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>22</v>
       </c>
@@ -1283,20 +1294,20 @@
       <c r="K7">
         <v>172776</v>
       </c>
-      <c r="L7">
-        <v>375777</v>
+      <c r="L7" s="2">
+        <v>0</v>
       </c>
       <c r="M7">
-        <v>6.0416670000000006E-2</v>
+        <v>0</v>
       </c>
       <c r="N7">
-        <v>5408742.1159530003</v>
+        <v>0</v>
       </c>
       <c r="O7">
-        <v>66278.723459999994</v>
-      </c>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>23</v>
       </c>
@@ -1330,17 +1341,17 @@
       <c r="K8">
         <v>122033</v>
       </c>
-      <c r="L8">
-        <v>32623</v>
+      <c r="L8" s="2">
+        <v>21659</v>
       </c>
       <c r="M8">
-        <v>3.159091E-2</v>
+        <v>9.6153799999999998E-3</v>
       </c>
       <c r="N8">
-        <v>1226129.90909</v>
+        <v>4983.398878</v>
       </c>
       <c r="O8">
-        <v>23004.958569999999</v>
+        <v>17253.547454</v>
       </c>
     </row>
   </sheetData>
@@ -1353,22 +1364,22 @@
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="18.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" t="s">
         <v>14</v>
       </c>
       <c r="C1" t="s">
@@ -1378,32 +1389,32 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2">
         <v>1</v>
       </c>
       <c r="B2">
         <v>17</v>
       </c>
       <c r="C2">
-        <v>231944.67664568662</v>
+        <v>2379.0207613499974</v>
       </c>
       <c r="D2">
         <v>178.41742500000001</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="2">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3">
         <v>2</v>
       </c>
       <c r="B3">
         <v>18</v>
       </c>
       <c r="C3">
-        <v>9984076.7464169022</v>
+        <v>325504.71863055689</v>
       </c>
       <c r="D3">
-        <v>1455.250951</v>
+        <v>4169.3476586995002</v>
       </c>
     </row>
   </sheetData>
@@ -1416,311 +1427,312 @@
   <dimension ref="A1:E17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="12" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="13.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="12.5703125" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="3" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2">
+      <c r="A2" s="3">
         <v>17</v>
       </c>
-      <c r="B2" t="s">
-        <v>23</v>
-      </c>
-      <c r="C2">
+      <c r="B2" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C2" s="3">
         <v>7.7499999999999999E-2</v>
       </c>
-      <c r="D2">
+      <c r="D2" s="3">
         <v>2.5024999999999999</v>
       </c>
-      <c r="E2">
+      <c r="E2" s="3">
         <f>D2*0.6</f>
         <v>1.5014999999999998</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3">
+      <c r="A3" s="3">
         <v>17</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C3" s="3">
+        <v>0.13</v>
+      </c>
+      <c r="D3" s="3">
+        <v>1.846666667</v>
+      </c>
+      <c r="E3" s="3">
+        <v>0.44323716600000002</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="3">
+        <v>17</v>
+      </c>
+      <c r="B4" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="C3">
-        <v>0.13</v>
-      </c>
-      <c r="D3">
-        <v>1.846666667</v>
-      </c>
-      <c r="E3">
-        <v>0.44323716600000002</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>17</v>
-      </c>
-      <c r="B4" t="s">
-        <v>25</v>
-      </c>
-      <c r="C4">
+      <c r="C4" s="3">
         <v>8.3992857000000004E-2</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="3">
         <v>0.98380449000000003</v>
       </c>
-      <c r="E4">
+      <c r="E4" s="3">
         <f>D4*0.6</f>
         <v>0.590282694</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5">
+      <c r="A5" s="3">
         <v>18</v>
       </c>
-      <c r="B5" t="s">
-        <v>23</v>
-      </c>
-      <c r="C5">
+      <c r="B5" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C5" s="3">
         <v>0.104</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="3">
         <v>1.2593333330000001</v>
       </c>
-      <c r="E5">
+      <c r="E5" s="3">
         <f>D5*0.6</f>
         <v>0.75559999980000003</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6">
+      <c r="A6" s="3">
         <v>18</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C6" s="3">
+        <v>0.140555556</v>
+      </c>
+      <c r="D6" s="3">
+        <v>1.795212732</v>
+      </c>
+      <c r="E6" s="3">
+        <v>0.41816441999999998</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="3">
+        <v>18</v>
+      </c>
+      <c r="B7" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="C6">
-        <v>0.140555556</v>
-      </c>
-      <c r="D6">
-        <v>1.795212732</v>
-      </c>
-      <c r="E6">
-        <v>0.41816441999999998</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>18</v>
-      </c>
-      <c r="B7" t="s">
-        <v>25</v>
-      </c>
-      <c r="C7">
+      <c r="C7" s="3">
         <v>8.4071434E-2</v>
       </c>
-      <c r="D7">
+      <c r="D7" s="3">
         <v>0.98553754800000004</v>
       </c>
-      <c r="E7">
+      <c r="E7" s="3">
         <f>D7*0.6</f>
         <v>0.59132252880000002</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8">
+      <c r="A8" s="3">
         <v>19</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C8" s="3">
+        <v>0.154</v>
+      </c>
+      <c r="D8" s="3">
+        <v>2.04</v>
+      </c>
+      <c r="E8" s="3">
+        <v>0.38100310199999998</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="3">
+        <v>19</v>
+      </c>
+      <c r="B9" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="C8">
-        <v>0.154</v>
-      </c>
-      <c r="D8">
-        <v>2.04</v>
-      </c>
-      <c r="E8">
-        <v>0.38100310199999998</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>19</v>
-      </c>
-      <c r="B9" t="s">
-        <v>25</v>
-      </c>
-      <c r="C9">
+      <c r="C9" s="3">
         <v>9.0518973000000003E-2</v>
       </c>
-      <c r="D9">
+      <c r="D9" s="3">
         <v>1.2294546129999999</v>
       </c>
-      <c r="E9">
+      <c r="E9" s="3">
         <f>D9*0.6</f>
         <v>0.73767276779999991</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10">
+      <c r="A10" s="3">
         <v>20</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C10" s="3">
+        <v>0.12842857099999999</v>
+      </c>
+      <c r="D10" s="3">
+        <v>1.929857143</v>
+      </c>
+      <c r="E10" s="3">
+        <v>0.44999999999999996</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="3">
+        <v>20</v>
+      </c>
+      <c r="B11" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="C10">
-        <v>0.12842857099999999</v>
-      </c>
-      <c r="D10">
-        <v>1.929857143</v>
-      </c>
-      <c r="E10">
-        <v>0.44999999999999996</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>20</v>
-      </c>
-      <c r="B11" t="s">
-        <v>25</v>
-      </c>
-      <c r="C11">
+      <c r="C11" s="3">
         <v>0.104666667</v>
       </c>
-      <c r="D11">
+      <c r="D11" s="3">
         <v>1.2633333330000001</v>
       </c>
-      <c r="E11">
+      <c r="E11" s="3">
         <f>D11*0.6</f>
         <v>0.75799999979999999</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12">
+      <c r="A12" s="3">
         <v>21</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C12" s="3">
+        <v>0.14676470599999999</v>
+      </c>
+      <c r="D12" s="3">
+        <v>1.9875084030000001</v>
+      </c>
+      <c r="E12" s="3">
+        <v>0.44999999999999996</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="3">
+        <v>21</v>
+      </c>
+      <c r="B13" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="C12">
-        <v>0.14676470599999999</v>
-      </c>
-      <c r="D12">
-        <v>1.9875084030000001</v>
-      </c>
-      <c r="E12">
-        <v>0.44999999999999996</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13">
-        <v>21</v>
-      </c>
-      <c r="B13" t="s">
-        <v>25</v>
-      </c>
-      <c r="C13">
+      <c r="C13" s="3">
         <v>0.100666667</v>
       </c>
-      <c r="D13">
+      <c r="D13" s="3">
         <v>1.2224888890000001</v>
       </c>
-      <c r="E13">
+      <c r="E13" s="3">
         <f>D13*0.6</f>
         <v>0.7334933334</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14">
+      <c r="A14" s="3">
         <v>22</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C14" s="3">
+        <v>0.13919797</v>
+      </c>
+      <c r="D14" s="3">
+        <v>1.802498731</v>
+      </c>
+      <c r="E14" s="3">
+        <v>0.44999999999999996</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="3">
+        <v>22</v>
+      </c>
+      <c r="B15" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="C14">
-        <v>0.13919797</v>
-      </c>
-      <c r="D14">
-        <v>1.802498731</v>
-      </c>
-      <c r="E14">
-        <v>0.44999999999999996</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15">
-        <v>22</v>
-      </c>
-      <c r="B15" t="s">
-        <v>25</v>
-      </c>
-      <c r="C15">
+      <c r="C15" s="3">
         <v>0.115166667</v>
       </c>
-      <c r="D15">
+      <c r="D15" s="3">
         <v>1.3866666670000001</v>
       </c>
-      <c r="E15">
+      <c r="E15" s="3">
         <f>D15*0.6</f>
         <v>0.83200000019999998</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16">
+      <c r="A16" s="3">
         <v>23</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B16" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C16" s="3">
+        <v>0.09</v>
+      </c>
+      <c r="D16" s="3">
+        <v>1.5</v>
+      </c>
+      <c r="E16" s="3">
+        <v>0.444230772</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="3">
+        <v>23</v>
+      </c>
+      <c r="B17" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="C16">
-        <v>0.09</v>
-      </c>
-      <c r="D16">
-        <v>1.5</v>
-      </c>
-      <c r="E16">
-        <v>0.444230772</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17">
-        <v>23</v>
-      </c>
-      <c r="B17" t="s">
-        <v>25</v>
-      </c>
-      <c r="C17">
+      <c r="C17" s="3">
         <v>9.6666666999999998E-2</v>
       </c>
-      <c r="D17">
+      <c r="D17" s="3">
         <v>1.1777777780000001</v>
       </c>
-      <c r="E17">
+      <c r="E17" s="3">
         <f>D17*0.6</f>
         <v>0.70666666680000001</v>
       </c>

</xml_diff>

<commit_message>
Changing ParentSoils concept to a generic Actions concept.
</commit_message>
<xml_diff>
--- a/cmd/cremexplorer/testdata/testInputExcelDataSet.xlsx
+++ b/cmd/cremexplorer/testdata/testInputExcelDataSet.xlsx
@@ -9,7 +9,7 @@
   <sheets>
     <sheet name="PlanningUnits" sheetId="1" r:id="rId1"/>
     <sheet name="Gullies" sheetId="2" r:id="rId2"/>
-    <sheet name="ParentSoils" sheetId="3" r:id="rId3"/>
+    <sheet name="Actions" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="145621"/>
   <extLst>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="27">
   <si>
     <t>Identifier</t>
   </si>
@@ -102,6 +102,9 @@
   </si>
   <si>
     <t>Gully</t>
+  </si>
+  <si>
+    <t>OpportunityCost</t>
   </si>
 </sst>
 </file>
@@ -946,7 +949,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1424,10 +1427,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E17"/>
+  <dimension ref="A1:F17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1436,10 +1439,11 @@
     <col min="2" max="2" width="10.42578125" style="3" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.85546875" style="3" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="13.7109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="12.5703125" style="3"/>
+    <col min="6" max="6" width="16" style="3" customWidth="1"/>
+    <col min="7" max="16384" width="12.5703125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>18</v>
       </c>
@@ -1455,8 +1459,11 @@
       <c r="E1" s="3" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
         <v>17</v>
       </c>
@@ -1473,8 +1480,11 @@
         <f>D2*0.6</f>
         <v>1.5014999999999998</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>17</v>
       </c>
@@ -1490,8 +1500,11 @@
       <c r="E3" s="3">
         <v>0.44323716600000002</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F3">
+        <v>11969.116740092626</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <v>17</v>
       </c>
@@ -1508,8 +1521,11 @@
         <f>D4*0.6</f>
         <v>0.590282694</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F4">
+        <v>6205.1723024022067</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
         <v>18</v>
       </c>
@@ -1526,8 +1542,11 @@
         <f>D5*0.6</f>
         <v>0.75559999980000003</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F5">
+        <v>317.83533591054601</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
         <v>18</v>
       </c>
@@ -1543,8 +1562,11 @@
       <c r="E6" s="3">
         <v>0.41816441999999998</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F6">
+        <v>72373.744154991917</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
         <v>18</v>
       </c>
@@ -1561,8 +1583,11 @@
         <f>D7*0.6</f>
         <v>0.59132252880000002</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F7">
+        <v>2236.700270436133</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
         <v>19</v>
       </c>
@@ -1578,8 +1603,11 @@
       <c r="E8" s="3">
         <v>0.38100310199999998</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F8">
+        <v>16368.774399517197</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
         <v>19</v>
       </c>
@@ -1596,8 +1624,11 @@
         <f>D9*0.6</f>
         <v>0.73767276779999991</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F9">
+        <v>1224.2486701957214</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
         <v>20</v>
       </c>
@@ -1613,8 +1644,11 @@
       <c r="E10" s="3">
         <v>0.44999999999999996</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
         <v>20</v>
       </c>
@@ -1631,8 +1665,11 @@
         <f>D11*0.6</f>
         <v>0.75799999979999999</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F11">
+        <v>3240.2366959041756</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="3">
         <v>21</v>
       </c>
@@ -1648,8 +1685,11 @@
       <c r="E12" s="3">
         <v>0.44999999999999996</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="3">
         <v>21</v>
       </c>
@@ -1666,8 +1706,11 @@
         <f>D13*0.6</f>
         <v>0.7334933334</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F13">
+        <v>3030.2103241448754</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="3">
         <v>22</v>
       </c>
@@ -1683,8 +1726,11 @@
       <c r="E14" s="3">
         <v>0.44999999999999996</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="3">
         <v>22</v>
       </c>
@@ -1701,8 +1747,11 @@
         <f>D15*0.6</f>
         <v>0.83200000019999998</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F15">
+        <v>2124.2628833762665</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="3">
         <v>23</v>
       </c>
@@ -1718,8 +1767,11 @@
       <c r="E16" s="3">
         <v>0.444230772</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F16">
+        <v>2.3919495589002002</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="3">
         <v>23</v>
       </c>
@@ -1735,6 +1787,9 @@
       <c r="E17" s="3">
         <f>D17*0.6</f>
         <v>0.70666666680000001</v>
+      </c>
+      <c r="F17">
+        <v>2925.5337950916137</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Implementing needed DissolvedNitrogen variable behaviour for current mgt actions.
</commit_message>
<xml_diff>
--- a/cmd/cremexplorer/testdata/testInputExcelDataSet.xlsx
+++ b/cmd/cremexplorer/testdata/testInputExcelDataSet.xlsx
@@ -11,6 +11,9 @@
     <sheet name="Gullies" sheetId="2" r:id="rId2"/>
     <sheet name="Actions" sheetId="3" r:id="rId3"/>
   </sheets>
+  <definedNames>
+    <definedName name="Actions" localSheetId="2">Actions!$A$1:$O$19</definedName>
+  </definedNames>
   <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -28,8 +31,34 @@
 </workbook>
 </file>
 
+<file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
+<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <connection id="1" name="Actions" type="6" refreshedVersion="4" background="1" saveData="1">
+    <textPr codePage="850" sourceFile="E:\Data\tmp\work\CREMExplorer_v0.14\input\Actions.csv" tab="0" comma="1">
+      <textFields count="15">
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
+</connections>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="34">
   <si>
     <t>Subcatchment</t>
   </si>
@@ -85,21 +114,6 @@
     <t>ImplementationCost</t>
   </si>
   <si>
-    <t>ParticulateNitrogenOriginal</t>
-  </si>
-  <si>
-    <t>ParticulateNitrogenActioned</t>
-  </si>
-  <si>
-    <t>HillslopeErosionOriginal</t>
-  </si>
-  <si>
-    <t>HillslopeErosionActioned</t>
-  </si>
-  <si>
-    <t>FineSedimentOriginal</t>
-  </si>
-  <si>
     <t>FineSedimentActioned</t>
   </si>
   <si>
@@ -110,6 +124,42 @@
   </si>
   <si>
     <t>Gully</t>
+  </si>
+  <si>
+    <t>ParticulateNitrogenOrigi0l</t>
+  </si>
+  <si>
+    <t>ParticulateNitroge0ctioned</t>
+  </si>
+  <si>
+    <t>HillslopeErosionOrigi0l</t>
+  </si>
+  <si>
+    <t>HillslopeErosio0ctioned</t>
+  </si>
+  <si>
+    <t>FineSedimentOrigi0l</t>
+  </si>
+  <si>
+    <t>DissolvedNitrogenOriginal</t>
+  </si>
+  <si>
+    <t>DissolvedNitrogenActioned</t>
+  </si>
+  <si>
+    <t>DNRemovalEfficiency</t>
+  </si>
+  <si>
+    <t>PNRemovalEfficiency</t>
+  </si>
+  <si>
+    <t>SedimentRemovalEfficiency</t>
+  </si>
+  <si>
+    <t>Wetland</t>
+  </si>
+  <si>
+    <t>wetland</t>
   </si>
 </sst>
 </file>
@@ -151,9 +201,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -169,6 +220,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Actions" connectionId="1" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -460,7 +515,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -861,27 +916,32 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J13"/>
+  <dimension ref="A1:O19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="L7" sqref="L7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="26.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="27.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="23" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="24" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="20.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="22" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="24.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="25.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="21.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="22.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="24.85546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="26" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="26.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -895,30 +955,45 @@
         <v>17</v>
       </c>
       <c r="E1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G1" t="s">
+        <v>24</v>
+      </c>
+      <c r="H1" t="s">
+        <v>25</v>
+      </c>
+      <c r="I1" t="s">
+        <v>26</v>
+      </c>
+      <c r="J1" t="s">
         <v>18</v>
       </c>
-      <c r="F1" t="s">
-        <v>19</v>
-      </c>
-      <c r="G1" t="s">
-        <v>20</v>
-      </c>
-      <c r="H1" t="s">
-        <v>21</v>
-      </c>
-      <c r="I1" t="s">
-        <v>22</v>
-      </c>
-      <c r="J1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K1" t="s">
+        <v>27</v>
+      </c>
+      <c r="L1" t="s">
+        <v>28</v>
+      </c>
+      <c r="M1" t="s">
+        <v>29</v>
+      </c>
+      <c r="N1" t="s">
+        <v>30</v>
+      </c>
+      <c r="O1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>17</v>
       </c>
       <c r="B2" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="C2">
         <v>0</v>
@@ -944,13 +1019,28 @@
       <c r="J2">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K2">
+        <v>1.01734E-4</v>
+      </c>
+      <c r="L2" s="2">
+        <v>4.57805E-5</v>
+      </c>
+      <c r="M2">
+        <v>0</v>
+      </c>
+      <c r="N2">
+        <v>0</v>
+      </c>
+      <c r="O2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>17</v>
       </c>
       <c r="B3" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="C3">
         <v>5449</v>
@@ -976,13 +1066,28 @@
       <c r="J3">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K3">
+        <v>1.564867679</v>
+      </c>
+      <c r="L3">
+        <v>1.489710283</v>
+      </c>
+      <c r="M3">
+        <v>0</v>
+      </c>
+      <c r="N3">
+        <v>0</v>
+      </c>
+      <c r="O3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>17</v>
       </c>
       <c r="B4" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="C4">
         <v>5722</v>
@@ -1008,13 +1113,28 @@
       <c r="J4">
         <v>0.14348038099999999</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K4" s="2">
+        <v>2.02556E-7</v>
+      </c>
+      <c r="L4" s="2">
+        <v>1.2364199999999999E-7</v>
+      </c>
+      <c r="M4">
+        <v>0.632175983</v>
+      </c>
+      <c r="N4">
+        <v>0</v>
+      </c>
+      <c r="O4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>18</v>
       </c>
       <c r="B5" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="C5">
         <v>0</v>
@@ -1040,13 +1160,28 @@
       <c r="J5">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K5">
+        <v>7.2399689999999997E-3</v>
+      </c>
+      <c r="L5">
+        <v>3.257958E-3</v>
+      </c>
+      <c r="M5">
+        <v>0</v>
+      </c>
+      <c r="N5">
+        <v>0</v>
+      </c>
+      <c r="O5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>18</v>
       </c>
       <c r="B6" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="C6">
         <v>96419</v>
@@ -1072,13 +1207,28 @@
       <c r="J6">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K6">
+        <v>5.2063129200000002</v>
+      </c>
+      <c r="L6">
+        <v>4.4223361729999997</v>
+      </c>
+      <c r="M6">
+        <v>0</v>
+      </c>
+      <c r="N6">
+        <v>0</v>
+      </c>
+      <c r="O6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>18</v>
       </c>
       <c r="B7" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="C7">
         <v>3801</v>
@@ -1104,13 +1254,28 @@
       <c r="J7">
         <v>0.185783848</v>
       </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K7" s="2">
+        <v>1.1853E-9</v>
+      </c>
+      <c r="L7" s="2">
+        <v>5.8785899999999997E-10</v>
+      </c>
+      <c r="M7">
+        <v>0.632175983</v>
+      </c>
+      <c r="N7">
+        <v>0</v>
+      </c>
+      <c r="O7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>19</v>
       </c>
       <c r="B8" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="C8">
         <v>4982</v>
@@ -1136,13 +1301,28 @@
       <c r="J8">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K8">
+        <v>2.9198410369999999</v>
+      </c>
+      <c r="L8">
+        <v>2.844638292</v>
+      </c>
+      <c r="M8">
+        <v>0</v>
+      </c>
+      <c r="N8">
+        <v>0</v>
+      </c>
+      <c r="O8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>19</v>
       </c>
       <c r="B9" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="C9">
         <v>698</v>
@@ -1168,133 +1348,490 @@
       <c r="J9">
         <v>0.16482466000000001</v>
       </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K9" s="2">
+        <v>2.1789099999999999E-10</v>
+      </c>
+      <c r="L9" s="2">
+        <v>1.2140599999999999E-10</v>
+      </c>
+      <c r="M9">
+        <v>0.632175983</v>
+      </c>
+      <c r="N9">
+        <v>0</v>
+      </c>
+      <c r="O9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>20</v>
       </c>
       <c r="B10" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="C10">
+        <v>0</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+      <c r="E10">
+        <v>0</v>
+      </c>
+      <c r="F10">
+        <v>0</v>
+      </c>
+      <c r="G10">
+        <v>0</v>
+      </c>
+      <c r="H10">
+        <v>0</v>
+      </c>
+      <c r="I10">
+        <v>0</v>
+      </c>
+      <c r="J10">
+        <v>0</v>
+      </c>
+      <c r="K10">
+        <v>2.2986143619999999</v>
+      </c>
+      <c r="L10">
+        <v>2.2161758530000002</v>
+      </c>
+      <c r="M10">
+        <v>0</v>
+      </c>
+      <c r="N10">
+        <v>0</v>
+      </c>
+      <c r="O10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>20</v>
+      </c>
+      <c r="B11" t="s">
+        <v>19</v>
+      </c>
+      <c r="C11">
         <v>1021</v>
       </c>
-      <c r="D10">
+      <c r="D11">
         <v>336288</v>
       </c>
-      <c r="E10">
-        <v>0</v>
-      </c>
-      <c r="F10">
-        <v>0</v>
-      </c>
-      <c r="G10">
-        <v>0</v>
-      </c>
-      <c r="H10">
-        <v>0</v>
-      </c>
-      <c r="I10">
+      <c r="E11">
+        <v>0</v>
+      </c>
+      <c r="F11">
+        <v>0</v>
+      </c>
+      <c r="G11">
+        <v>0</v>
+      </c>
+      <c r="H11">
+        <v>0</v>
+      </c>
+      <c r="I11">
         <v>0.178053397</v>
       </c>
-      <c r="J10">
+      <c r="J11">
         <v>0.21527084799999999</v>
       </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11">
+      <c r="K11" s="2">
+        <v>3.01917E-8</v>
+      </c>
+      <c r="L11" s="2">
+        <v>1.6070300000000001E-8</v>
+      </c>
+      <c r="M11">
+        <v>0.632175983</v>
+      </c>
+      <c r="N11">
+        <v>0</v>
+      </c>
+      <c r="O11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A12">
         <v>21</v>
       </c>
-      <c r="B11" t="s">
-        <v>24</v>
-      </c>
-      <c r="C11">
-        <v>0</v>
-      </c>
-      <c r="D11">
+      <c r="B12" t="s">
+        <v>20</v>
+      </c>
+      <c r="C12">
+        <v>0</v>
+      </c>
+      <c r="D12">
+        <v>0</v>
+      </c>
+      <c r="E12">
+        <v>0</v>
+      </c>
+      <c r="F12">
+        <v>0</v>
+      </c>
+      <c r="G12">
+        <v>0</v>
+      </c>
+      <c r="H12">
+        <v>0</v>
+      </c>
+      <c r="I12">
+        <v>0</v>
+      </c>
+      <c r="J12">
+        <v>0</v>
+      </c>
+      <c r="K12">
+        <v>3.113707303</v>
+      </c>
+      <c r="L12">
+        <v>2.996628512</v>
+      </c>
+      <c r="M12">
+        <v>0</v>
+      </c>
+      <c r="N12">
+        <v>0</v>
+      </c>
+      <c r="O12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>21</v>
+      </c>
+      <c r="B13" t="s">
+        <v>19</v>
+      </c>
+      <c r="C13">
+        <v>0</v>
+      </c>
+      <c r="D13">
         <v>463369</v>
       </c>
-      <c r="E11">
-        <v>0</v>
-      </c>
-      <c r="F11">
-        <v>0</v>
-      </c>
-      <c r="G11">
-        <v>0</v>
-      </c>
-      <c r="H11">
-        <v>0</v>
-      </c>
-      <c r="I11">
+      <c r="E13">
+        <v>0</v>
+      </c>
+      <c r="F13">
+        <v>0</v>
+      </c>
+      <c r="G13">
+        <v>0</v>
+      </c>
+      <c r="H13">
+        <v>0</v>
+      </c>
+      <c r="I13">
         <v>0.157850089</v>
       </c>
-      <c r="J11">
+      <c r="J13">
         <v>0.20331195099999999</v>
       </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12">
+      <c r="K13" s="2">
+        <v>1.7060700000000001E-9</v>
+      </c>
+      <c r="L13" s="2">
+        <v>9.23323E-10</v>
+      </c>
+      <c r="M13">
+        <v>0.632175983</v>
+      </c>
+      <c r="N13">
+        <v>0</v>
+      </c>
+      <c r="O13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>21</v>
+      </c>
+      <c r="B14" t="s">
+        <v>33</v>
+      </c>
+      <c r="C14">
+        <v>19177</v>
+      </c>
+      <c r="D14">
+        <v>1392717</v>
+      </c>
+      <c r="E14">
+        <v>0</v>
+      </c>
+      <c r="F14">
+        <v>0</v>
+      </c>
+      <c r="G14">
+        <v>0</v>
+      </c>
+      <c r="H14">
+        <v>0</v>
+      </c>
+      <c r="I14">
+        <v>0</v>
+      </c>
+      <c r="J14">
+        <v>0</v>
+      </c>
+      <c r="K14">
+        <v>0</v>
+      </c>
+      <c r="L14">
+        <v>0</v>
+      </c>
+      <c r="M14">
+        <v>0.99</v>
+      </c>
+      <c r="N14">
+        <v>1</v>
+      </c>
+      <c r="O14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A15">
         <v>22</v>
       </c>
-      <c r="B12" t="s">
-        <v>24</v>
-      </c>
-      <c r="C12">
+      <c r="B15" t="s">
+        <v>20</v>
+      </c>
+      <c r="C15">
+        <v>0</v>
+      </c>
+      <c r="D15">
+        <v>0</v>
+      </c>
+      <c r="E15">
+        <v>0</v>
+      </c>
+      <c r="F15">
+        <v>0</v>
+      </c>
+      <c r="G15">
+        <v>0</v>
+      </c>
+      <c r="H15">
+        <v>0</v>
+      </c>
+      <c r="I15">
+        <v>0</v>
+      </c>
+      <c r="J15">
+        <v>0</v>
+      </c>
+      <c r="K15">
+        <v>4.6665866649999996</v>
+      </c>
+      <c r="L15">
+        <v>4.3980503669999997</v>
+      </c>
+      <c r="M15">
+        <v>0</v>
+      </c>
+      <c r="N15">
+        <v>0</v>
+      </c>
+      <c r="O15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>22</v>
+      </c>
+      <c r="B16" t="s">
+        <v>19</v>
+      </c>
+      <c r="C16">
         <v>6522</v>
       </c>
-      <c r="D12">
+      <c r="D16">
         <v>829324</v>
       </c>
-      <c r="E12">
-        <v>0</v>
-      </c>
-      <c r="F12">
-        <v>0</v>
-      </c>
-      <c r="G12">
-        <v>0</v>
-      </c>
-      <c r="H12">
-        <v>0</v>
-      </c>
-      <c r="I12">
+      <c r="E16">
+        <v>0</v>
+      </c>
+      <c r="F16">
+        <v>0</v>
+      </c>
+      <c r="G16">
+        <v>0</v>
+      </c>
+      <c r="H16">
+        <v>0</v>
+      </c>
+      <c r="I16">
         <v>0.13776703600000001</v>
       </c>
-      <c r="J12">
+      <c r="J16">
         <v>0.19665379799999999</v>
       </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13">
+      <c r="K16" s="2">
+        <v>8.5303499999999997E-11</v>
+      </c>
+      <c r="L16" s="2">
+        <v>4.4089500000000002E-11</v>
+      </c>
+      <c r="M16">
+        <v>0.632175983</v>
+      </c>
+      <c r="N16">
+        <v>0</v>
+      </c>
+      <c r="O16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>22</v>
+      </c>
+      <c r="B17" t="s">
+        <v>32</v>
+      </c>
+      <c r="C17">
+        <v>6331</v>
+      </c>
+      <c r="D17">
+        <v>2451354</v>
+      </c>
+      <c r="E17">
+        <v>0</v>
+      </c>
+      <c r="F17">
+        <v>0</v>
+      </c>
+      <c r="G17">
+        <v>0</v>
+      </c>
+      <c r="H17">
+        <v>0</v>
+      </c>
+      <c r="I17">
+        <v>0</v>
+      </c>
+      <c r="J17">
+        <v>0</v>
+      </c>
+      <c r="K17">
+        <v>0</v>
+      </c>
+      <c r="L17">
+        <v>0</v>
+      </c>
+      <c r="M17">
+        <v>0.98</v>
+      </c>
+      <c r="N17">
+        <v>1</v>
+      </c>
+      <c r="O17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A18">
         <v>23</v>
       </c>
-      <c r="B13" t="s">
-        <v>24</v>
-      </c>
-      <c r="C13">
+      <c r="B18" t="s">
+        <v>20</v>
+      </c>
+      <c r="C18">
+        <v>0</v>
+      </c>
+      <c r="D18">
+        <v>0</v>
+      </c>
+      <c r="E18">
+        <v>0</v>
+      </c>
+      <c r="F18">
+        <v>0</v>
+      </c>
+      <c r="G18">
+        <v>0</v>
+      </c>
+      <c r="H18">
+        <v>0</v>
+      </c>
+      <c r="I18">
+        <v>0</v>
+      </c>
+      <c r="J18">
+        <v>0</v>
+      </c>
+      <c r="K18">
+        <v>1.180786796</v>
+      </c>
+      <c r="L18">
+        <v>1.133323598</v>
+      </c>
+      <c r="M18">
+        <v>0</v>
+      </c>
+      <c r="N18">
+        <v>0</v>
+      </c>
+      <c r="O18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>23</v>
+      </c>
+      <c r="B19" t="s">
+        <v>19</v>
+      </c>
+      <c r="C19">
         <v>3292</v>
       </c>
-      <c r="D13">
+      <c r="D19">
         <v>585757</v>
       </c>
-      <c r="E13">
-        <v>0</v>
-      </c>
-      <c r="F13">
-        <v>0</v>
-      </c>
-      <c r="G13">
-        <v>0</v>
-      </c>
-      <c r="H13">
-        <v>0</v>
-      </c>
-      <c r="I13">
+      <c r="E19">
+        <v>0</v>
+      </c>
+      <c r="F19">
+        <v>0</v>
+      </c>
+      <c r="G19">
+        <v>0</v>
+      </c>
+      <c r="H19">
+        <v>0</v>
+      </c>
+      <c r="I19">
         <v>0.13346128199999999</v>
       </c>
-      <c r="J13">
+      <c r="J19">
         <v>0.204580122</v>
+      </c>
+      <c r="K19" s="2">
+        <v>1.3322700000000001E-7</v>
+      </c>
+      <c r="L19" s="2">
+        <v>6.4536700000000001E-8</v>
+      </c>
+      <c r="M19">
+        <v>0.632175983</v>
+      </c>
+      <c r="N19">
+        <v>0</v>
+      </c>
+      <c r="O19">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -1306,6 +1843,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100EC5899B031002D4AB69421D85EAB54C4" ma:contentTypeVersion="9" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="273db2e2a0b4d1a84e6184e572e09e18">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="06deb609-ee1b-41e8-876b-59c28e07861f" xmlns:ns4="8398cf50-eaa3-435c-afa6-f6d15ce00c08" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="5d387e558b917f5e4819b73100bceb62" ns3:_="" ns4:_="">
     <xsd:import namespace="06deb609-ee1b-41e8-876b-59c28e07861f"/>
@@ -1502,12 +2045,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -1518,6 +2055,23 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{94ED0015-E867-4612-9CB8-2A837E95A83C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="8398cf50-eaa3-435c-afa6-f6d15ce00c08"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="06deb609-ee1b-41e8-876b-59c28e07861f"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9B22DF29-A939-435B-AF62-6B4E71867B7E}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1536,23 +2090,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{94ED0015-E867-4612-9CB8-2A837E95A83C}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="06deb609-ee1b-41e8-876b-59c28e07861f"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="8398cf50-eaa3-435c-afa6-f6d15ce00c08"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{59516B63-6103-4841-AE24-CD8BD7D94BF2}">
   <ds:schemaRefs>

</xml_diff>